<commit_message>
Feat(JDT): Remplissage du journal de travail
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_BamertMathieu.xlsx
+++ b/Doc/Journal-de-Travail_BamertMathieu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv23aha\Documents\GitHub\Todo-DevOps-Test\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0BE034-B2E6-423E-AECC-CAC04AC707EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BB2D03-EE74-4F4B-B834-22AEC957418D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -131,6 +131,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Discussion du projet</t>
+  </si>
+  <si>
+    <t>Mise en place du projet</t>
+  </si>
+  <si>
+    <t>Création du planning</t>
+  </si>
+  <si>
+    <t>Remplissage du journal de travail</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1169,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2012,7 +2024,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4198,7 +4210,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4251,7 +4263,7 @@
       <c r="B3" s="87"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>0 heures 0 minutes</v>
+        <v>1 heures 30 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4264,15 +4276,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4307,27 +4319,45 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="str">
+      <c r="A7" s="61">
         <f>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</f>
-        <v/>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="23"/>
+        <v>46</v>
+      </c>
+      <c r="B7" s="26">
+        <v>45974</v>
+      </c>
+      <c r="C7" s="27">
+        <v>1</v>
+      </c>
+      <c r="D7" s="28">
+        <v>10</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>30</v>
+      </c>
       <c r="G7" s="38"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="62" t="str">
+      <c r="A8" s="62">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v/>
-      </c>
-      <c r="B8" s="30"/>
+        <v>46</v>
+      </c>
+      <c r="B8" s="30">
+        <v>45974</v>
+      </c>
       <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="23"/>
+      <c r="D8" s="32">
+        <v>5</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>31</v>
+      </c>
       <c r="G8" s="39"/>
       <c r="M8" t="s">
         <v>15</v>
@@ -4340,15 +4370,23 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="str">
+      <c r="A9" s="63">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="34"/>
+        <v>46</v>
+      </c>
+      <c r="B9" s="34">
+        <v>45974</v>
+      </c>
       <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="23"/>
+      <c r="D9" s="36">
+        <v>10</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="G9" s="40"/>
       <c r="M9" t="s">
         <v>16</v>
@@ -4361,15 +4399,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="str">
+      <c r="A10" s="62">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="30"/>
+        <v>46</v>
+      </c>
+      <c r="B10" s="30">
+        <v>45974</v>
+      </c>
       <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="23"/>
+      <c r="D10" s="32">
+        <v>5</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>33</v>
+      </c>
       <c r="G10" s="39"/>
       <c r="M10" t="s">
         <v>17</v>
@@ -10850,9 +10896,9 @@
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
         <v>0 h 00 min</v>
       </c>
-      <c r="G6" s="72" t="e">
+      <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10887,9 +10933,9 @@
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
         <v>0 h 00 min</v>
       </c>
-      <c r="G7" s="75" t="e">
+      <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10924,9 +10970,9 @@
         <f t="shared" si="1"/>
         <v>0 h 00 min</v>
       </c>
-      <c r="G8" s="72" t="e">
+      <c r="G8" s="72">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L8" s="54" t="str">
         <f>'Journal de travail'!M10</f>
@@ -10943,15 +10989,15 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10959,11 +11005,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 00 min</v>
-      </c>
-      <c r="G9" s="75" t="e">
+        <v>1 h 30 min</v>
+      </c>
+      <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10997,9 +11043,9 @@
         <f t="shared" ref="F10" si="4">QUOTIENT(SUM(A10:B10),60)&amp;" h "&amp;TEXT(MOD(SUM(A10:B10),60), "00")&amp;" min"</f>
         <v>0 h 00 min</v>
       </c>
-      <c r="G10" s="80" t="e">
+      <c r="G10" s="80">
         <f>SUM(A10:B10)/$C$11</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L10" s="69" t="s">
         <v>18</v>
@@ -11015,26 +11061,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 00 min</v>
+        <v>1 h 30 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0</v>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>
@@ -11078,6 +11124,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e12e7c6bdfb75a7d9b849cfc56f051f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd34f7c8cce3bbcb7db5b2c1b48d4341" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11272,15 +11327,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11293,6 +11339,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4B38329-2CCE-448E-AD8B-127B28816FC3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11311,14 +11365,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Feat(JDT): Remplissage de mon journal de travail
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_BamertMathieu.xlsx
+++ b/Doc/Journal-de-Travail_BamertMathieu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv23aha\Documents\GitHub\Todo-DevOps-Test\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BB2D03-EE74-4F4B-B834-22AEC957418D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B056E9B5-0822-4171-834D-AD5D4C64EBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -143,6 +143,24 @@
   </si>
   <si>
     <t>Remplissage du journal de travail</t>
+  </si>
+  <si>
+    <t>Création des tâches dans github project</t>
+  </si>
+  <si>
+    <t>Déployement de l'application</t>
+  </si>
+  <si>
+    <t>Tester l'application en testant toutes les fonctionnalités</t>
+  </si>
+  <si>
+    <t>Trouver les bugs de l'application</t>
+  </si>
+  <si>
+    <t>J'ai commencé le rapport</t>
+  </si>
+  <si>
+    <t>Discussion de ce qu'on va faire avec Yosef</t>
   </si>
 </sst>
 </file>
@@ -1163,13 +1181,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2018,13 +2036,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.3829787234042548E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.34042553191489361</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.5957446808510638</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4210,7 +4228,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4263,7 +4281,7 @@
       <c r="B3" s="87"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 30 minutes</v>
+        <v>3 heures 55 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4276,15 +4294,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>30</v>
+        <v>115</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>90</v>
+        <v>235</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4428,15 +4446,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="str">
+      <c r="A11" s="63">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="34"/>
+        <v>47</v>
+      </c>
+      <c r="B11" s="34">
+        <v>45981</v>
+      </c>
       <c r="C11" s="35"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="23"/>
+      <c r="D11" s="36">
+        <v>25</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="G11" s="40"/>
       <c r="M11" t="s">
         <v>14</v>
@@ -4449,15 +4475,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="str">
+      <c r="A12" s="62">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="B12" s="30">
+        <v>45981</v>
+      </c>
       <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="23"/>
+      <c r="D12" s="32">
+        <v>15</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>35</v>
+      </c>
       <c r="G12" s="39"/>
       <c r="M12" t="s">
         <v>18</v>
@@ -4470,15 +4504,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="str">
+      <c r="A13" s="63">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="34"/>
+        <v>47</v>
+      </c>
+      <c r="B13" s="34">
+        <v>45981</v>
+      </c>
       <c r="C13" s="35"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="23"/>
+      <c r="D13" s="36">
+        <v>10</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>36</v>
+      </c>
       <c r="G13" s="40"/>
       <c r="N13">
         <v>6</v>
@@ -4488,15 +4530,25 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="str">
+      <c r="A14" s="62">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="23"/>
+        <v>47</v>
+      </c>
+      <c r="B14" s="30">
+        <v>45981</v>
+      </c>
+      <c r="C14" s="31">
+        <v>1</v>
+      </c>
+      <c r="D14" s="32">
+        <v>10</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>37</v>
+      </c>
       <c r="G14" s="39"/>
       <c r="N14">
         <v>7</v>
@@ -4506,15 +4558,23 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="str">
+      <c r="A15" s="63">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="34"/>
+        <v>47</v>
+      </c>
+      <c r="B15" s="34">
+        <v>45981</v>
+      </c>
       <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="23"/>
+      <c r="D15" s="36">
+        <v>10</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>38</v>
+      </c>
       <c r="G15" s="40"/>
       <c r="N15">
         <v>8</v>
@@ -4524,30 +4584,46 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="str">
+      <c r="A16" s="62">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="B16" s="30">
+        <v>45981</v>
+      </c>
       <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="23"/>
+      <c r="D16" s="32">
+        <v>5</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>33</v>
+      </c>
       <c r="G16" s="39"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="str">
+      <c r="A17" s="63">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="34"/>
+        <v>48</v>
+      </c>
+      <c r="B17" s="34">
+        <v>45985</v>
+      </c>
       <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="23"/>
+      <c r="D17" s="36">
+        <v>10</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>39</v>
+      </c>
       <c r="G17" s="40"/>
       <c r="O17">
         <v>45</v>
@@ -10919,11 +10995,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10931,11 +11007,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
+        <v>0 h 15 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0</v>
+        <v>6.3829787234042548E-2</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10952,15 +11028,15 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E8,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E8" s="76" t="str">
         <f>'Journal de travail'!M10</f>
@@ -10968,11 +11044,11 @@
       </c>
       <c r="F8" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 00 min</v>
+        <v>1 h 20 min</v>
       </c>
       <c r="G8" s="72">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.34042553191489361</v>
       </c>
       <c r="L8" s="54" t="str">
         <f>'Journal de travail'!M10</f>
@@ -10993,11 +11069,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11005,11 +11081,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 30 min</v>
+        <v>2 h 20 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5957446808510638</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11061,26 +11137,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>30</v>
+        <v>115</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>90</v>
+        <v>235</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 30 min</v>
+        <v>3 h 55 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>1.6666666666666666E-2</v>
+        <v>4.3518518518518519E-2</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Feat(JDT): Remplissage du JDT
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_BamertMathieu.xlsx
+++ b/Doc/Journal-de-Travail_BamertMathieu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pv23aha\Documents\GitHub\Todo-DevOps-Test\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B056E9B5-0822-4171-834D-AD5D4C64EBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC0263F-2BC8-4D29-877B-5340FE6084E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>Discussion de ce qu'on va faire avec Yosef</t>
+  </si>
+  <si>
+    <t>Remplissage de la partie spécification et plannification initial</t>
+  </si>
+  <si>
+    <t>Remplissage de la partie classification de bugs</t>
+  </si>
+  <si>
+    <t>Suppresion de fichier inutile</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1196,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2036,13 +2045,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3829787234042548E-2</c:v>
+                  <c:v>4.6153846153846156E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34042553191489361</c:v>
+                  <c:v>0.24615384615384617</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5957446808510638</c:v>
+                  <c:v>0.70769230769230773</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4228,7 +4237,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4281,7 +4290,7 @@
       <c r="B3" s="87"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>3 heures 55 minutes</v>
+        <v>5 heures 25 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4298,11 +4307,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>115</v>
+        <v>205</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>235</v>
+        <v>325</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4630,57 +4639,89 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="str">
+      <c r="A18" s="62">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="B18" s="30">
+        <v>45985</v>
+      </c>
       <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="23"/>
+      <c r="D18" s="32">
+        <v>50</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>40</v>
+      </c>
       <c r="G18" s="39"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="str">
+      <c r="A19" s="63">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="34"/>
+        <v>48</v>
+      </c>
+      <c r="B19" s="34">
+        <v>45985</v>
+      </c>
       <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="36">
+        <v>30</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="G19" s="40"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="62" t="str">
+      <c r="A20" s="62">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="30"/>
+        <v>48</v>
+      </c>
+      <c r="B20" s="30">
+        <v>45985</v>
+      </c>
       <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="23"/>
+      <c r="D20" s="32">
+        <v>5</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>42</v>
+      </c>
       <c r="G20" s="39"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="str">
+      <c r="A21" s="63">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="34"/>
+        <v>48</v>
+      </c>
+      <c r="B21" s="34">
+        <v>45985</v>
+      </c>
       <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="23"/>
+      <c r="D21" s="36">
+        <v>5</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>33</v>
+      </c>
       <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -11011,7 +11052,7 @@
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>6.3829787234042548E-2</v>
+        <v>4.6153846153846156E-2</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11048,7 +11089,7 @@
       </c>
       <c r="G8" s="72">
         <f t="shared" si="2"/>
-        <v>0.34042553191489361</v>
+        <v>0.24615384615384617</v>
       </c>
       <c r="L8" s="54" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11069,11 +11110,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>230</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11081,11 +11122,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 20 min</v>
+        <v>3 h 50 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.5957446808510638</v>
+        <v>0.70769230769230773</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11141,22 +11182,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>115</v>
+        <v>205</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>235</v>
+        <v>325</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>3 h 55 min</v>
+        <v>5 h 25 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>4.3518518518518519E-2</v>
+        <v>6.0185185185185182E-2</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>29</v>

</xml_diff>